<commit_message>
pue utilization in dos scenarios (research study)
</commit_message>
<xml_diff>
--- a/simulation_reports/dos/dos.xlsx
+++ b/simulation_reports/dos/dos.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vemanuele/Documents/GitHub/masters-degree-thesis/simulation_reports/dos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E95023FA-4353-2440-8E13-58EF18C54E94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B9D602-7799-2A4B-B898-E802A6513326}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="980" windowWidth="26840" windowHeight="14820" xr2:uid="{F534D240-4720-1D41-89DF-E24DA06CAE5D}"/>
+    <workbookView xWindow="1960" yWindow="980" windowWidth="26840" windowHeight="14820" xr2:uid="{F534D240-4720-1D41-89DF-E24DA06CAE5D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -120,7 +120,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>DoS Scenario (PUE)</a:t>
+              <a:t>Fast DoS Scenario (PUE)</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -5230,8 +5230,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4CBAD2B-51D1-9941-BEB5-6BE671C63748}">
   <dimension ref="A1:C656"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" activeCellId="1" sqref="A1:A1048576 C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A583" workbookViewId="0">
+      <selection activeCell="C210" sqref="C210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>